<commit_message>
Add Tests and Plots
</commit_message>
<xml_diff>
--- a/PythonEnvironment/resources/mutations_FEW.xlsx
+++ b/PythonEnvironment/resources/mutations_FEW.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelprobst/Desktop/thesis/Scavenger/PythonEnvironment/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\_Thesis\Scavenger\PythonEnvironment\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8FB57D-7089-4ECB-B8B8-44D5E6889ADA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -126,7 +127,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -170,7 +171,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -207,457 +207,15 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0697706752869817"/>
+          <c:x val="6.9770675286981707E-2"/>
           <c:y val="0.111036263111729"/>
-          <c:w val="0.792962730622963"/>
+          <c:w val="0.79296273062296296"/>
           <c:h val="0.773254861969355"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
-              <c:strCache>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Notes</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Method</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$51</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>0.483333333333333</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.566666666666666</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.666666666666666</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.566666666666666</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.749999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.666666666666666</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.683333333333333</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.683333333333333</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.633333333333333</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.666666666666666</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.516666666666666</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.733333333333333</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.566666666666666</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.583333333333333</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.383333333333333</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.566666666666666</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.633333333333333</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.416666666666666</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.483333333333333</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.733333333333333</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.616666666666666</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.516666666666666</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-34E1-4A86-BB4E-3659B33EE1F8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.05</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
-              <c:strCache>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Notes</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Method</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$51</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>0.24</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.28</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.229999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.19</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.219999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.439999999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.229999999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.47</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.329999999999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.339999999999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.52</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.56</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.67</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.49</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.61</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.48</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.57</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.97</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.59</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.659999999999999</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-34E1-4A86-BB4E-3659B33EE1F8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
@@ -807,13 +365,13 @@
                   <c:v>0.38</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.329999999999999</c:v>
+                  <c:v>0.32999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.329999999999999</c:v>
+                  <c:v>0.32999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.36</c:v>
@@ -822,10 +380,10 @@
                   <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.55</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.679999999999999</c:v>
+                  <c:v>0.67999999999999905</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.62</c:v>
@@ -852,13 +410,13 @@
                   <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.919999999999999</c:v>
+                  <c:v>0.91999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.459999999999999</c:v>
+                  <c:v>0.45999999999999902</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.919999999999999</c:v>
+                  <c:v>0.91999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0.83</c:v>
@@ -867,457 +425,15 @@
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-34E1-4A86-BB4E-3659B33EE1F8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.01</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
-              <c:strCache>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Notes</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Method</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$2:$E$51</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>0.24</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.269999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.28</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.329999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.269999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.28</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.28</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.27</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.31</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.319999999999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.43</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.46</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.48</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.539999999999999</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.62</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.62</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.789999999999999</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.59</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-34E1-4A86-BB4E-3659B33EE1F8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>lin decay</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
-              <c:strCache>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Notes</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Method</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$F$2:$F$51</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>0.24</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.229999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.27</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.36</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.279999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.36</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.41</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.269999999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.46</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.329999999999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.26</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.61</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.63</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.72</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.63</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.63</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.76</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.77</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-34E1-4A86-BB4E-3659B33EE1F8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1464,7 +580,7 @@
                   <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.29</c:v>
+                  <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.41</c:v>
@@ -1497,7 +613,7 @@
                   <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.58</c:v>
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.59</c:v>
@@ -1509,7 +625,7 @@
                   <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.76</c:v>
@@ -1518,7 +634,7 @@
                   <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.57</c:v>
+                  <c:v>0.56999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0.869999999999999</c:v>
@@ -1533,12 +649,17 @@
                   <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.57</c:v>
+                  <c:v>0.56999999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-42D1-4AC2-B66D-6361D497AC62}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -1704,13 +825,13 @@
                   <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.56</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.49</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.57</c:v>
+                  <c:v>0.56999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.86</c:v>
@@ -1728,13 +849,13 @@
                   <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.58</c:v>
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.679999999999999</c:v>
+                  <c:v>0.67999999999999905</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.55</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>0.61</c:v>
@@ -1752,225 +873,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>fit-based</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
-              <c:strCache>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Notes</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Method</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$I$2:$I$51</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>0.24</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.27</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.38</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.21</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.28</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.27</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.42</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.28</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.58</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.19</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.26</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-42D1-4AC2-B66D-6361D497AC62}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1982,12 +889,1224 @@
         </c:dLbls>
         <c:axId val="1825239184"/>
         <c:axId val="1824579376"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>0.1</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$51</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>Notes</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>Method</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$2:$B$51</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>0.483333333333333</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.56666666666666599</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.66666666666666596</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.56666666666666599</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.749999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.66666666666666596</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.68333333333333302</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.68333333333333302</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.65</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.63333333333333297</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.66666666666666596</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.51666666666666605</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.73333333333333295</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.56666666666666599</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.58333333333333304</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.38333333333333303</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.56666666666666599</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.63333333333333297</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0.41666666666666602</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.483333333333333</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>0.73333333333333295</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.61666666666666603</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>0.51666666666666605</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-34E1-4A86-BB4E-3659B33EE1F8}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>0.05</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$51</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>Notes</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>Method</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$2:$C$51</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>0.24</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.16</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.28000000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.22999999999999901</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.19</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.219999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.11</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.439999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.22999999999999901</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.3</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.47</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.32999999999999902</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.33999999999999903</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.52</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.56000000000000005</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.67</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.49</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.61</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.48</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.56999999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0.45</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.97</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>0.59</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.65999999999999903</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-34E1-4A86-BB4E-3659B33EE1F8}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>0.01</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$51</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>Notes</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>Method</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$2:$E$51</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>0.24</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.26999999999999902</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.28000000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.32999999999999902</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.26999999999999902</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.21</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.25</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.28000000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.28000000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.27</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.31</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.32</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.31999999999999901</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.45</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.43</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.46</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.48</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.53999999999999904</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.62</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0.62</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.78999999999999904</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>0.59</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.7</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>0.84</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-34E1-4A86-BB4E-3659B33EE1F8}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>lin decay</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$51</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>Notes</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>Method</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$2:$F$51</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>0.24</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.22999999999999901</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.27</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.22</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.36</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.2</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.27999999999999903</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.36</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.41</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.26999999999999902</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.46</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.32999999999999902</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.3</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.45</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.45</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.26</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.61</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.4</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.63</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.72</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0.63</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.63</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>0.76</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.77</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>0.85</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-34E1-4A86-BB4E-3659B33EE1F8}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="7"/>
+                <c:order val="7"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$I$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>fit-based</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$51</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="27"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>Notes</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>Method</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$I$2:$I$51</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>0.24</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.27</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.38</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.21</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.25</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.24</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.28000000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.27</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.13</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.22</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.22</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.42</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.28000000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.22</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.3</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.22</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.2</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.64</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0.57999999999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.19</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>0.26</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.16</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>0.12</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-42D1-4AC2-B66D-6361D497AC62}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="1825239184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="25.0"/>
+          <c:max val="25"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2031,7 +2150,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2106,7 +2224,7 @@
         <c:axId val="1824579376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2150,7 +2268,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2231,7 +2348,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2874,7 +2990,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3157,16 +3273,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H26"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3195,7 +3311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3224,7 +3340,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3253,7 +3369,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3282,7 +3398,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3311,7 +3427,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3340,7 +3456,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3369,7 +3485,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3398,7 +3514,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3427,7 +3543,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3456,7 +3572,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3485,7 +3601,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3514,7 +3630,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3543,7 +3659,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3572,7 +3688,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3601,7 +3717,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3630,7 +3746,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3659,7 +3775,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3688,7 +3804,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3717,7 +3833,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3746,7 +3862,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3775,7 +3891,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3804,7 +3920,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3833,7 +3949,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3862,7 +3978,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3891,7 +4007,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3920,7 +4036,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -3940,7 +4056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>

</xml_diff>